<commit_message>
SIS2 Part2 KUMARBEK MAGZHAN SIS2302
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -8,53 +8,75 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68FAC2A4-F561-47AF-8AB2-9A52245B52AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441C5A3E-D1A7-4E85-94AE-CDEEE4669E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{555A6DD0-9178-4B00-9E3B-6EA32AE7F260}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Updated Students" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Current.S</t>
-  </si>
-  <si>
-    <t>New.S</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Scholarship</t>
   </si>
   <si>
     <t>Ermek</t>
   </si>
   <si>
+    <t>eng-2401</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
     <t>Khadisha</t>
   </si>
   <si>
+    <t>eco-2405</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
     <t>Bekzhan</t>
   </si>
   <si>
+    <t>phy-2415</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
     <t>Arystan</t>
+  </si>
+  <si>
+    <t>mrk-2424</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>gpa</t>
+  </si>
+  <si>
+    <t>faculty</t>
+  </si>
+  <si>
+    <t>newScholarship</t>
   </si>
 </sst>
 </file>
@@ -64,10 +86,9 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -406,68 +427,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5020912E-4317-4A92-8303-55A3C07A2BC8}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>21021</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2">
+        <v>41898</v>
+      </c>
+      <c r="E2">
+        <v>2.79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>41898</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>23023</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>41898</v>
       </c>
-      <c r="C2">
-        <v>47168</v>
+      <c r="E3">
+        <v>3.01</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>41898</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>41898</v>
-      </c>
-      <c r="C3">
-        <v>47168</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>25025</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>63000</v>
+      </c>
+      <c r="E4">
+        <v>2.83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>63000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>63000</v>
-      </c>
-      <c r="C4">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>27027</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
         <v>67000</v>
       </c>
-      <c r="C5">
-        <v>73000</v>
+      <c r="E5">
+        <v>3.14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>67000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>